<commit_message>
View Register script updated
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-ViewRegister.xlsx
+++ b/tests/artifact/script/UI-ViewRegister.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="18350" windowHeight="6920" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -57,12 +57,25 @@
     <definedName name="javaui">'#system'!$N$2:$N$16</definedName>
     <definedName name="browserstack">'#system'!$G$2:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="813">
   <si>
     <t>target</t>
   </si>
@@ -2334,6 +2347,9 @@
   </si>
   <si>
     <t>${org.hamburger}</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
   <si>
     <t>click on Reports</t>
@@ -2504,12 +2520,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -2601,6 +2617,61 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -2609,6 +2680,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2624,114 +2734,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2740,6 +2742,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2766,67 +2782,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2844,7 +2806,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2856,79 +2938,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2940,7 +2956,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2990,26 +3006,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3038,6 +3054,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3053,17 +3084,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3078,158 +3103,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3275,14 +3291,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3458,52 +3474,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -6497,7 +6513,7 @@
   <dimension ref="A1:O188"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -9827,10 +9843,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O179"/>
+  <dimension ref="A1:O180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -10002,12 +10018,14 @@
         <v>30</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>363</v>
+        <v>576</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>756</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="27" t="s">
+        <v>757</v>
+      </c>
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
@@ -10018,46 +10036,46 @@
       <c r="N6" s="48"/>
       <c r="O6" s="47"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="7" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A7" s="19"/>
-      <c r="B7" s="30" t="s">
-        <v>757</v>
-      </c>
+      <c r="B7" s="30"/>
       <c r="C7" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>363</v>
+        <v>715</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="22"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="47"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A8" s="19"/>
       <c r="B8" s="30" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>363</v>
+        <v>576</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>760</v>
-      </c>
-      <c r="F8" s="27"/>
+        <v>759</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>757</v>
+      </c>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
@@ -10069,22 +10087,22 @@
       <c r="O8" s="22"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A9" s="19" t="s">
-        <v>761</v>
-      </c>
+      <c r="A9" s="19"/>
       <c r="B9" s="30" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>253</v>
+        <v>576</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>763</v>
-      </c>
-      <c r="F9" s="28"/>
+        <v>761</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>757</v>
+      </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
@@ -10096,9 +10114,11 @@
       <c r="O9" s="22"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A10" s="19"/>
+      <c r="A10" s="19" t="s">
+        <v>762</v>
+      </c>
       <c r="B10" s="30" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>30</v>
@@ -10107,7 +10127,7 @@
         <v>253</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="27"/>
@@ -10123,20 +10143,18 @@
     <row r="11" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A11" s="19"/>
       <c r="B11" s="30" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>692</v>
+        <v>253</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>767</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>768</v>
-      </c>
+        <v>766</v>
+      </c>
+      <c r="F11" s="28"/>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
@@ -10149,18 +10167,20 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A12" s="19"/>
-      <c r="B12" s="30"/>
+      <c r="B12" s="30" t="s">
+        <v>767</v>
+      </c>
       <c r="C12" s="26" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>656</v>
+        <v>692</v>
       </c>
       <c r="E12" s="27" t="s">
+        <v>768</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>769</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>770</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
@@ -10174,19 +10194,19 @@
     </row>
     <row r="13" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A13" s="19"/>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>656</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>770</v>
+      </c>
+      <c r="F13" s="28" t="s">
         <v>771</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>772</v>
-      </c>
-      <c r="F13" s="28"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
@@ -10199,17 +10219,17 @@
     </row>
     <row r="14" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="19"/>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="31" t="s">
+        <v>772</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>773</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>774</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="27"/>
@@ -10225,20 +10245,18 @@
     <row r="15" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A15" s="19"/>
       <c r="B15" s="30" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>707</v>
+        <v>253</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>774</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>776</v>
-      </c>
+        <v>775</v>
+      </c>
+      <c r="F15" s="28"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
@@ -10252,18 +10270,20 @@
     <row r="16" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="19"/>
       <c r="B16" s="30" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>253</v>
+        <v>707</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>778</v>
-      </c>
-      <c r="F16" s="28"/>
+        <v>775</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>777</v>
+      </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
@@ -10277,20 +10297,18 @@
     <row r="17" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="19"/>
       <c r="B17" s="30" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>707</v>
+        <v>253</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>780</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>781</v>
-      </c>
+        <v>779</v>
+      </c>
+      <c r="F17" s="28"/>
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
       <c r="I17" s="27"/>
@@ -10304,18 +10322,20 @@
     <row r="18" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="19"/>
       <c r="B18" s="30" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>363</v>
+        <v>707</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>783</v>
-      </c>
-      <c r="F18" s="28"/>
+        <v>781</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>782</v>
+      </c>
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
@@ -10329,16 +10349,16 @@
     <row r="19" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="19"/>
       <c r="B19" s="30" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>253</v>
+        <v>363</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="27"/>
@@ -10354,16 +10374,16 @@
     <row r="20" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A20" s="19"/>
       <c r="B20" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>363</v>
+        <v>253</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" s="27"/>
@@ -10379,16 +10399,16 @@
     <row r="21" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="19"/>
       <c r="B21" s="30" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>253</v>
+        <v>363</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="27"/>
@@ -10403,21 +10423,19 @@
     </row>
     <row r="22" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="19"/>
-      <c r="B22" s="31" t="s">
-        <v>790</v>
+      <c r="B22" s="30" t="s">
+        <v>789</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>483</v>
+        <v>253</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>791</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>792</v>
-      </c>
+        <v>790</v>
+      </c>
+      <c r="F22" s="28"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
@@ -10430,20 +10448,20 @@
     </row>
     <row r="23" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="19"/>
-      <c r="B23" s="30" t="s">
-        <v>793</v>
+      <c r="B23" s="31" t="s">
+        <v>791</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
@@ -10457,20 +10475,20 @@
     </row>
     <row r="24" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="19"/>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="30" t="s">
+        <v>794</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>493</v>
+      </c>
+      <c r="E24" s="27" t="s">
         <v>795</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>465</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>796</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>797</v>
+      <c r="F24" s="28" t="s">
+        <v>793</v>
       </c>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
@@ -10484,20 +10502,20 @@
     </row>
     <row r="25" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="19"/>
-      <c r="B25" s="30" t="s">
-        <v>798</v>
+      <c r="B25" s="20" t="s">
+        <v>796</v>
       </c>
       <c r="C25" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="37" t="s">
-        <v>49</v>
+      <c r="D25" s="35" t="s">
+        <v>465</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>799</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>800</v>
+        <v>797</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>798</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
@@ -10512,19 +10530,19 @@
     <row r="26" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A26" s="19"/>
       <c r="B26" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>800</v>
+      </c>
+      <c r="F26" s="27" t="s">
         <v>801</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>302</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>802</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>803</v>
       </c>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
@@ -10539,19 +10557,19 @@
     <row r="27" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A27" s="19"/>
       <c r="B27" s="30" t="s">
+        <v>802</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>803</v>
+      </c>
+      <c r="F27" s="36" t="s">
         <v>804</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>493</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>805</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>806</v>
       </c>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
@@ -10566,19 +10584,19 @@
     <row r="28" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="19"/>
       <c r="B28" s="30" t="s">
+        <v>805</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>493</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>806</v>
+      </c>
+      <c r="F28" s="28" t="s">
         <v>807</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>471</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>808</v>
-      </c>
-      <c r="F28" s="28" t="s">
-        <v>809</v>
       </c>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
@@ -10593,7 +10611,7 @@
     <row r="29" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A29" s="19"/>
       <c r="B29" s="30" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C29" s="34" t="s">
         <v>5</v>
@@ -10602,10 +10620,10 @@
         <v>471</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
@@ -10619,11 +10637,21 @@
     </row>
     <row r="30" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A30" s="19"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="28"/>
+      <c r="B30" s="30" t="s">
+        <v>811</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>471</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>809</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>812</v>
+      </c>
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
@@ -10636,11 +10664,11 @@
     </row>
     <row r="31" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="26"/>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
@@ -13167,6 +13195,23 @@
       <c r="N179" s="23"/>
       <c r="O179" s="22"/>
     </row>
+    <row r="180" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A180" s="19"/>
+      <c r="B180" s="20"/>
+      <c r="C180" s="26"/>
+      <c r="D180" s="27"/>
+      <c r="E180" s="27"/>
+      <c r="F180" s="27"/>
+      <c r="G180" s="27"/>
+      <c r="H180" s="27"/>
+      <c r="I180" s="27"/>
+      <c r="J180" s="50"/>
+      <c r="K180" s="22"/>
+      <c r="L180" s="23"/>
+      <c r="M180" s="21"/>
+      <c r="N180" s="23"/>
+      <c r="O180" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
@@ -13174,18 +13219,18 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N80:N179">
+  <conditionalFormatting sqref="N81:N180">
     <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N80,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N81,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N80,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N81,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N80,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N81,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N3:N79">
+  <conditionalFormatting sqref="N1 N3:N80">
     <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -13197,10 +13242,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C14 C15 C16 C17 C18 C21 C22 C23 C26 C27 C28 C29 C30 C12:C13 C19:C20 C24:C25 C31:C179">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C15 C16 C17 C18 C19 C22 C23 C24 C27 C28 C29 C30 C31 C13:C14 C20:C21 C25:C26 C32:C180">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D14 D15 D16 D17 D18 D21 D22 D23 D26 D27 D28 D29 D30 D12:D13 D19:D20 D24:D25 D31:D179">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D15 D16 D17 D18 D19 D22 D23 D24 D27 D28 D29 D30 D31 D13:D14 D20:D21 D25:D26 D32:D180">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>